<commit_message>
Reserve serial numbers of the work order position
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>spr_id</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>The Serial Number is error, can't find the s/n in current work order s/n reservation list.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_qc_1001</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Serial Number is error, can't find in goods receipt serial number list(OSRN)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列号输入错误，不在对应的采购收货序列号(OSRN)列表中</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1024,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1101,16 +1113,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1121,10 +1133,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -1135,10 +1147,38 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Release for Solution / Proposal, Prototype
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>spr_id</t>
   </si>
@@ -93,6 +93,28 @@
   </si>
   <si>
     <t>序列号输入错误，不在对应的采购收货序列号(OSRN)列表中</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_qc_1002</t>
+  </si>
+  <si>
+    <t>The input Serial Number is ok.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列号输入正确</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_qc_1003</t>
+  </si>
+  <si>
+    <t>The &lt;dw_1.item.qs_id.value&gt; of S/N(&lt;parent.dw_1.item.udf1.value&gt;) updated.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列号(&lt;parent.dw_1.item.udf1.value&gt;)的&lt;dw_1.item.qs_id.value&gt;已经更新</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1036,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1127,30 +1149,30 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -1161,10 +1183,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -1175,10 +1197,66 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Release for Prototype - bug fix
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>spr_id</t>
   </si>
@@ -115,6 +115,17 @@
   </si>
   <si>
     <t>序列号(&lt;parent.dw_1.item.udf1.value&gt;)的&lt;dw_1.item.qs_id.value&gt;已经更新</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_qc_1004</t>
+  </si>
+  <si>
+    <t>Can't edit the qc position of this sample, please input the correct serial number.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>不能输入该样品的质检项目，请输入正确的序列号</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1058,17 +1069,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -1177,16 +1188,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -1197,10 +1208,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -1211,10 +1222,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -1225,10 +1236,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -1239,10 +1250,10 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -1253,10 +1264,38 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HBAS Phase II Interim 1A by Will & 2A
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>spr_id</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>序列号输入错误，该样品状态为“已解锁”</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_wo_1002</t>
+  </si>
+  <si>
+    <t>beas_wo_1002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成品收货的序列号&lt;dw_1.item.serialnumber.value&gt;，没有找到对应的原料序列号</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The serial number of finish goods &lt;dw_1.item.serialnumber.value&gt;, did not find the match raw material's serial number</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1080,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1135,10 +1150,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -1149,10 +1164,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1163,10 +1178,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1177,10 +1192,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -1191,10 +1206,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -1205,10 +1220,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -1219,24 +1234,24 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -1247,10 +1262,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -1261,10 +1276,10 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -1275,10 +1290,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -1289,10 +1304,10 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -1303,10 +1318,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -1317,10 +1332,10 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -1331,9 +1346,37 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E19" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HBAS ERP Trial Production before unit test
Before unit testing in my pc
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>spr_id</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t xml:space="preserve">CH  </t>
-  </si>
-  <si>
-    <t>NULL</t>
   </si>
   <si>
     <t xml:space="preserve">E   </t>
@@ -132,14 +129,6 @@
     <t>beas_qc_1005</t>
   </si>
   <si>
-    <t>The input Serial Number is error, the sample status is unlocked.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列号输入错误，该样品状态为“已解锁”</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>beas_wo_1002</t>
   </si>
   <si>
@@ -152,6 +141,57 @@
   </si>
   <si>
     <t>The serial number of finish goods &lt;dw_1.item.serialnumber.value&gt;, did not find the match raw material's serial number</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列号输入错误，该样品状态必须为“打开”</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The input Serial Number is error, the sample status must be Open.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_tr_1003</t>
+  </si>
+  <si>
+    <t>beas_tr_1002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列号输入错误，不在工作令现有相关序列号管理物料的已发出序列号列表中</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Serial Number is error, can't find the s/n in current work order related serial management item goods issue.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">E   </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Warehouse cost indicator is "1-Must be zero"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_md_1001</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The warehouse set "1-Must be zero", the cost price always be 0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_md_1002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓库成本标记为“1-必须为0”</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓库成本标记为“1-必须为0”，成本单价总是为 0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1095,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1132,252 +1172,264 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
       <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1401,7 +1453,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HBAS ERP Trial Production release for BPP
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>spr_id</t>
   </si>
@@ -192,6 +192,20 @@
   </si>
   <si>
     <t>仓库成本标记为“1-必须为0”，成本单价总是为 0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_qc_1006</t>
+  </si>
+  <si>
+    <t>S/N entered cannot be duplicated in one QC order</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_qc_1007</t>
+  </si>
+  <si>
+    <t>S/N is mandatory.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1135,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1412,23 +1426,45 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
         <v>45</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update & fix bug for VCCT1 on 2014.9.1
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18180" windowHeight="9900"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15480" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="error message" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
   <si>
     <t>spr_id</t>
   </si>
@@ -285,17 +285,71 @@
   <si>
     <t>不能打开测量窗口，请检查序列号</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_tr_1004</t>
+  </si>
+  <si>
+    <t>beas_tr_1005</t>
+  </si>
+  <si>
+    <t>The cost element is mandatory.</t>
+  </si>
+  <si>
+    <t>You enter the S/N, therefore the confirmed quantity cannot be more than 1</t>
+  </si>
+  <si>
+    <t>The time type is "Proc. 01", therefore cannot input the quantity.</t>
+  </si>
+  <si>
+    <t>beas_tr_1006</t>
+  </si>
+  <si>
+    <t>beas_mm_1001</t>
+  </si>
+  <si>
+    <t>&lt;dw_1.item.itemcode.value&gt;-&lt;dw_1.item.itemname.value&gt; cannot maintain in this screen</t>
+  </si>
+  <si>
+    <t>&lt;cuser&gt;,you have no right to open item master data window the screen will be close!</t>
+  </si>
+  <si>
+    <t>beas_mm_1002</t>
+  </si>
+  <si>
+    <t>This item can NOT maintain in this screen</t>
+  </si>
+  <si>
+    <t>beas_mm_1003</t>
+  </si>
+  <si>
+    <t>The Standard evaluation only</t>
+  </si>
+  <si>
+    <t>beas_mm_1004</t>
+  </si>
+  <si>
+    <t>The unit name in Inventory Tab is mandatory information for inventory item</t>
+  </si>
+  <si>
+    <t>beas_mm_1005</t>
+  </si>
+  <si>
+    <t>This item cost must great than 0, else it will be block in Transaction document</t>
+  </si>
+  <si>
+    <t>beas_mm_1006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -303,7 +357,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -312,7 +366,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -321,7 +375,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -330,7 +384,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -339,7 +393,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -347,7 +401,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -355,7 +409,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -363,7 +417,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -371,7 +425,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -380,7 +434,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -389,7 +443,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -397,7 +451,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -406,7 +460,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -414,7 +468,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -423,7 +477,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -432,7 +486,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -440,14 +494,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -887,48 +941,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -941,7 +995,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1227,20 +1281,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1271,7 +1325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1336,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1293,7 +1347,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1304,7 +1358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1315,411 +1369,543 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>48</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
         <v>61</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
         <v>65</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
         <v>11</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
         <v>12</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
         <v>15</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
         <v>37</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
         <v>18</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
         <v>21</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
         <v>24</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
         <v>27</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
         <v>30</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
         <v>48</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
         <v>50</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
         <v>52</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E41" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
         <v>54</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E42" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
         <v>57</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E43" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
         <v>59</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
         <v>60</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E45" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
         <v>61</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
         <v>65</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
         <v>41</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C48" t="s">
         <v>43</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E48" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
         <v>41</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C49" t="s">
         <v>45</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E49" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>88</v>
+      </c>
+      <c r="E53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1736,12 +1922,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="67.625" customWidth="1"/>
+    <col min="1" max="1" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="27" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" ht="30">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update for VCCT1 on 2014.9.12
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="15480" windowHeight="9900"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="115">
   <si>
     <t>spr_id</t>
   </si>
@@ -339,17 +339,98 @@
   </si>
   <si>
     <t>beas_mm_1006</t>
+  </si>
+  <si>
+    <t>beas_tr_1007</t>
+  </si>
+  <si>
+    <t>The "From Date" and the "Valuation Date" must be same.</t>
+  </si>
+  <si>
+    <t>beas_wo_1003</t>
+  </si>
+  <si>
+    <t>The receipt quantity can't greater than total issue quantity</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_wo_1003</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>退货数量不得大于发货数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成本要素为必填项</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果输入了序列号, 那么确认数量不得大于 1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"开始日期"和"计价日期"必须一致</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间类型为 "Proc. 01", 不得输入数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_wo_1004</t>
+  </si>
+  <si>
+    <t>The S/N or B/N is error, can't find the s/n in current work order related item goods issue.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can't receipt assembly for this work order position, some operation sequences still open</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_wo_1005</t>
+  </si>
+  <si>
+    <t>The S/N or B/N is error, can't find the s/n in current work order related item goods receipt.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beas_wo_1006</t>
+  </si>
+  <si>
+    <t>beas_wo_1007</t>
+  </si>
+  <si>
+    <t>The batch management item receipt quantity can't greater than total issue quantity</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列号或批号错误, 无法在已发出的发料单中，找到相应的批号或序列号</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>此工作令的部分工序仍然为“打开”，所以无法做成品收货</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列号或批号错误, 无法在已收到的收料单中，找到相应的批号或序列号.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>批号管理物料的退货数量不得大于发货数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -357,7 +438,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -366,7 +447,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -375,7 +456,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -384,7 +465,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -393,7 +474,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -401,7 +482,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -409,7 +490,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -417,7 +498,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -425,7 +506,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -434,7 +515,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -443,7 +524,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -451,7 +532,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -460,7 +541,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -468,7 +549,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -477,7 +558,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -486,7 +567,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -494,14 +575,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -941,48 +1022,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -995,7 +1076,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1281,20 +1362,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1325,7 +1406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1336,575 +1417,707 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>75</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
         <v>76</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E43" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
         <v>80</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E44" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
         <v>24</v>
       </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
         <v>27</v>
       </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
         <v>30</v>
       </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
         <v>50</v>
       </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
         <v>52</v>
       </c>
-      <c r="E17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
         <v>54</v>
       </c>
-      <c r="E18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="E54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
         <v>57</v>
       </c>
-      <c r="E19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="E55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
         <v>59</v>
       </c>
-      <c r="E20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="E56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
         <v>60</v>
       </c>
-      <c r="E21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
         <v>61</v>
       </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
         <v>65</v>
       </c>
-      <c r="E23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" t="s">
         <v>43</v>
       </c>
-      <c r="E24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" t="s">
         <v>45</v>
       </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" t="s">
-        <v>59</v>
-      </c>
-      <c r="E44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>65</v>
-      </c>
-      <c r="E47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="E61" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
         <v>81</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E62" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
         <v>84</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E63" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
         <v>86</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E64" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
         <v>88</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E65" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
         <v>90</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E66" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
         <v>92</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E67" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1922,12 +2135,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="67.5703125" customWidth="1"/>
+    <col min="1" max="1" width="67.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30">
+    <row r="1" spans="1:1" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update for VCCT1 on 2014.9.14
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="15480" windowHeight="9900"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="117">
   <si>
     <t>spr_id</t>
   </si>
@@ -420,17 +420,23 @@
   <si>
     <t>批号管理物料的退货数量不得大于发货数量</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The "warehouse cost" and "consignment vendor" of "from warehouse" and "to warehouse" fields must be same.</t>
+  </si>
+  <si>
+    <t>beas_mm_1007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -438,7 +444,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -447,7 +453,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -456,7 +462,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -465,7 +471,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -474,7 +480,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -482,7 +488,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -490,7 +496,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -498,7 +504,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -506,7 +512,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -515,7 +521,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -524,7 +530,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -532,7 +538,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -541,7 +547,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -549,7 +555,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -558,7 +564,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -567,7 +573,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -575,14 +581,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1022,48 +1028,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1076,7 +1082,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1362,20 +1368,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1417,7 +1423,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1450,7 +1456,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1467,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1494,7 +1500,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1505,7 +1511,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1560,7 +1566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1593,7 +1599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1648,7 +1654,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1659,7 +1665,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1681,7 +1687,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1703,7 +1709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1725,400 +1731,488 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>7</v>
       </c>
       <c r="C32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
         <v>11</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
         <v>31</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
         <v>97</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E41" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
         <v>103</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E42" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
         <v>106</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E43" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
         <v>108</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E44" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
         <v>109</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E45" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
         <v>12</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E46" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
         <v>15</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
         <v>37</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E48" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
         <v>75</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E49" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
         <v>76</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E50" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" t="s">
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
         <v>80</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E51" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
         <v>93</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E52" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
         <v>18</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
         <v>21</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E54" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
         <v>24</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E55" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
         <v>27</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E56" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s">
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
         <v>30</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E57" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
         <v>48</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E58" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
         <v>50</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
         <v>52</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E60" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s">
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
         <v>54</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E61" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
         <v>57</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E62" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
         <v>59</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E63" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
         <v>60</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s">
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
         <v>61</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
         <v>65</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" t="s">
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
         <v>41</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C67" t="s">
         <v>43</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E67" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
         <v>41</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C68" t="s">
         <v>45</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E68" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s">
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
         <v>81</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E69" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s">
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
         <v>84</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E70" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s">
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
         <v>86</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E71" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
         <v>88</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
         <v>90</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E73" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s">
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
         <v>92</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E74" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>116</v>
+      </c>
+      <c r="E75" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2135,12 +2229,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="67.625" customWidth="1"/>
+    <col min="1" max="1" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="27" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" ht="30">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
VCCT 3 of SBO_SP_TransactionNotification
</commit_message>
<xml_diff>
--- a/error message.xlsx
+++ b/error message.xlsx
@@ -1370,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>